<commit_message>
💄logo footer date changes
</commit_message>
<xml_diff>
--- a/dist/SDS/report.xlsx
+++ b/dist/SDS/report.xlsx
@@ -31,13 +31,19 @@
     <t>AMOUNT</t>
   </si>
   <si>
-    <t>01/15/2024</t>
-  </si>
-  <si>
-    <t>01/14/2024</t>
-  </si>
-  <si>
-    <t>01/07/2024</t>
+    <t>07/01/2024</t>
+  </si>
+  <si>
+    <t>14/01/2024</t>
+  </si>
+  <si>
+    <t>15/01/2024</t>
+  </si>
+  <si>
+    <t>Malinao, Nica Ella</t>
+  </si>
+  <si>
+    <t>Pandino, Daniela Nicole</t>
   </si>
   <si>
     <t>Lopez, Harvey</t>
@@ -46,103 +52,97 @@
     <t>Artista, Chrillian</t>
   </si>
   <si>
+    <t>Dianzo, Adrian Lloyd</t>
+  </si>
+  <si>
+    <t>Mijares, Aliza Love</t>
+  </si>
+  <si>
+    <t>Yaiso, Donie</t>
+  </si>
+  <si>
+    <t>Celaje, Raven</t>
+  </si>
+  <si>
+    <t>Francisco, Carlos</t>
+  </si>
+  <si>
+    <t>Tejero, Roxanne</t>
+  </si>
+  <si>
+    <t>Gomez, Angelica</t>
+  </si>
+  <si>
+    <t>Borrel, Joven</t>
+  </si>
+  <si>
+    <t>Balamban, Kieth Jasmien</t>
+  </si>
+  <si>
+    <t>Monje, Mieke Shaine</t>
+  </si>
+  <si>
+    <t>Del Castillo, Patricia</t>
+  </si>
+  <si>
+    <t>Lucban, Hershey Mae</t>
+  </si>
+  <si>
+    <t>Mora, Sean Ivan</t>
+  </si>
+  <si>
     <t>Asilo, Chrishalene</t>
   </si>
   <si>
-    <t>Borrel, Joven</t>
-  </si>
-  <si>
-    <t>Celaje, Raven</t>
+    <t>Reotutar, Samantha</t>
+  </si>
+  <si>
+    <t>Sombilla, Daisery</t>
+  </si>
+  <si>
+    <t>Nagales, Luis Angelo</t>
   </si>
   <si>
     <t>Curativo, Methel</t>
   </si>
   <si>
-    <t>Dianzo, Adrian Lloyd</t>
-  </si>
-  <si>
     <t>Encinas, Jason</t>
   </si>
   <si>
-    <t>Francisco, Carlos</t>
-  </si>
-  <si>
-    <t>Gomez, Angelica</t>
-  </si>
-  <si>
-    <t>Lucban, Hershey Mae</t>
-  </si>
-  <si>
-    <t>Malinao, Nica Ella</t>
-  </si>
-  <si>
-    <t>Mijares, Aliza Love</t>
-  </si>
-  <si>
-    <t>Monje, Mieke Shaine</t>
-  </si>
-  <si>
-    <t>Mora, Sean Ivan</t>
-  </si>
-  <si>
-    <t>Nagales, Luis Angelo</t>
-  </si>
-  <si>
-    <t>Pandino, Daniela Nicole</t>
-  </si>
-  <si>
-    <t>Reotutar, Samantha</t>
-  </si>
-  <si>
     <t>Sarmiento, Jessa</t>
   </si>
   <si>
-    <t>Sombilla, Daisery</t>
-  </si>
-  <si>
-    <t>Tejero, Roxanne</t>
-  </si>
-  <si>
-    <t>Yaiso, Donie</t>
-  </si>
-  <si>
-    <t>Balamban, Kieth Jasmien</t>
-  </si>
-  <si>
-    <t>Del Castillo, Patricia</t>
-  </si>
-  <si>
     <t>Transpo</t>
   </si>
   <si>
+    <t>Load, Transpo</t>
+  </si>
+  <si>
+    <t>Transpo, Load</t>
+  </si>
+  <si>
+    <t>Load, Project, Transpo</t>
+  </si>
+  <si>
     <t>Transpo, Uniform</t>
   </si>
   <si>
     <t>Transpo, Project</t>
   </si>
   <si>
-    <t>Transpo, Load</t>
+    <t>Transpo, SSS</t>
+  </si>
+  <si>
+    <t>Transpo, Fees</t>
   </si>
   <si>
     <t>OJT</t>
   </si>
   <si>
-    <t>Transpo, SSS</t>
-  </si>
-  <si>
-    <t>Load, Project, Transpo</t>
-  </si>
-  <si>
-    <t>Transpo, Fees</t>
-  </si>
-  <si>
-    <t>Load, Transpo</t>
+    <t>This is a description</t>
   </si>
   <si>
     <t>this is a description</t>
-  </si>
-  <si>
-    <t>This is a description</t>
   </si>
   <si>
     <t>January 2024 EXPENSES</t>
@@ -624,7 +624,7 @@
         <v>41</v>
       </c>
       <c r="F6" s="7">
-        <v>200</v>
+        <v>156</v>
       </c>
     </row>
     <row r="7" spans="2:6" ht="22" customHeight="1">
@@ -632,44 +632,46 @@
         <v>6</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>32</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="7">
-        <v>240</v>
+        <v>156</v>
       </c>
     </row>
     <row r="8" spans="2:6" ht="22" customHeight="1">
       <c r="B8" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="7">
-        <v>654</v>
+        <v>172</v>
       </c>
     </row>
     <row r="9" spans="2:6" ht="22" customHeight="1">
       <c r="B9" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="6"/>
+      <c r="E9" s="6" t="s">
+        <v>42</v>
+      </c>
       <c r="F9" s="7">
-        <v>430</v>
+        <v>200</v>
       </c>
     </row>
     <row r="10" spans="2:6" ht="22" customHeight="1">
@@ -677,14 +679,14 @@
         <v>6</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>32</v>
       </c>
       <c r="E10" s="6"/>
       <c r="F10" s="7">
-        <v>310</v>
+        <v>240</v>
       </c>
     </row>
     <row r="11" spans="2:6" ht="22" customHeight="1">
@@ -692,14 +694,14 @@
         <v>6</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E11" s="6"/>
       <c r="F11" s="7">
-        <v>737</v>
+        <v>252</v>
       </c>
     </row>
     <row r="12" spans="2:6" ht="22" customHeight="1">
@@ -707,14 +709,14 @@
         <v>6</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="7">
-        <v>252</v>
+        <v>292</v>
       </c>
     </row>
     <row r="13" spans="2:6" ht="22" customHeight="1">
@@ -722,14 +724,14 @@
         <v>6</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E13" s="6"/>
       <c r="F13" s="7">
-        <v>737</v>
+        <v>300</v>
       </c>
     </row>
     <row r="14" spans="2:6" ht="22" customHeight="1">
@@ -737,14 +739,14 @@
         <v>6</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>32</v>
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="7">
-        <v>330</v>
+        <v>300</v>
       </c>
     </row>
     <row r="15" spans="2:6" ht="22" customHeight="1">
@@ -752,29 +754,29 @@
         <v>6</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>32</v>
       </c>
       <c r="E15" s="6"/>
       <c r="F15" s="7">
-        <v>420</v>
+        <v>310</v>
       </c>
     </row>
     <row r="16" spans="2:6" ht="22" customHeight="1">
       <c r="B16" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>32</v>
       </c>
       <c r="E16" s="6"/>
       <c r="F16" s="7">
-        <v>462</v>
+        <v>330</v>
       </c>
     </row>
     <row r="17" spans="2:6" ht="22" customHeight="1">
@@ -782,29 +784,29 @@
         <v>6</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E17" s="6"/>
       <c r="F17" s="7">
-        <v>565</v>
+        <v>330</v>
       </c>
     </row>
     <row r="18" spans="2:6" ht="22" customHeight="1">
       <c r="B18" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>32</v>
       </c>
       <c r="E18" s="6"/>
       <c r="F18" s="7">
-        <v>156</v>
+        <v>350</v>
       </c>
     </row>
     <row r="19" spans="2:6" ht="22" customHeight="1">
@@ -812,14 +814,14 @@
         <v>6</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>32</v>
       </c>
       <c r="E19" s="6"/>
       <c r="F19" s="7">
-        <v>300</v>
+        <v>357</v>
       </c>
     </row>
     <row r="20" spans="2:6" ht="22" customHeight="1">
@@ -827,14 +829,14 @@
         <v>6</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>32</v>
       </c>
       <c r="E20" s="6"/>
       <c r="F20" s="7">
-        <v>646</v>
+        <v>420</v>
       </c>
     </row>
     <row r="21" spans="2:6" ht="22" customHeight="1">
@@ -842,14 +844,14 @@
         <v>6</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E21" s="6"/>
       <c r="F21" s="7">
-        <v>585</v>
+        <v>430</v>
       </c>
     </row>
     <row r="22" spans="2:6" ht="22" customHeight="1">
@@ -857,440 +859,438 @@
         <v>6</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E22" s="6"/>
       <c r="F22" s="7">
-        <v>680</v>
+        <v>462</v>
       </c>
     </row>
     <row r="23" spans="2:6" ht="22" customHeight="1">
       <c r="B23" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E23" s="6"/>
       <c r="F23" s="7">
-        <v>292</v>
+        <v>490</v>
       </c>
     </row>
     <row r="24" spans="2:6" ht="22" customHeight="1">
       <c r="B24" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>32</v>
       </c>
       <c r="E24" s="6"/>
       <c r="F24" s="7">
-        <v>625</v>
+        <v>490</v>
       </c>
     </row>
     <row r="25" spans="2:6" ht="22" customHeight="1">
       <c r="B25" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E25" s="6"/>
+        <v>32</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>41</v>
+      </c>
       <c r="F25" s="7">
-        <v>750</v>
+        <v>510</v>
       </c>
     </row>
     <row r="26" spans="2:6" ht="22" customHeight="1">
       <c r="B26" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="E26" s="6"/>
       <c r="F26" s="7">
-        <v>677</v>
+        <v>513</v>
       </c>
     </row>
     <row r="27" spans="2:6" ht="22" customHeight="1">
       <c r="B27" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E27" s="6"/>
+      <c r="E27" s="6" t="s">
+        <v>41</v>
+      </c>
       <c r="F27" s="7">
-        <v>357</v>
+        <v>528</v>
       </c>
     </row>
     <row r="28" spans="2:6" ht="22" customHeight="1">
       <c r="B28" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D28" s="6" t="s">
         <v>32</v>
       </c>
       <c r="E28" s="6"/>
       <c r="F28" s="7">
-        <v>300</v>
+        <v>528</v>
       </c>
     </row>
     <row r="29" spans="2:6" ht="22" customHeight="1">
       <c r="B29" s="5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E29" s="6"/>
       <c r="F29" s="7">
-        <v>584</v>
+        <v>536</v>
       </c>
     </row>
     <row r="30" spans="2:6" ht="22" customHeight="1">
       <c r="B30" s="5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E30" s="6"/>
       <c r="F30" s="7">
-        <v>490</v>
+        <v>540</v>
       </c>
     </row>
     <row r="31" spans="2:6" ht="22" customHeight="1">
       <c r="B31" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E31" s="6"/>
       <c r="F31" s="7">
-        <v>760</v>
+        <v>565</v>
       </c>
     </row>
     <row r="32" spans="2:6" ht="22" customHeight="1">
       <c r="B32" s="5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E32" s="6"/>
       <c r="F32" s="7">
-        <v>513</v>
+        <v>584</v>
       </c>
     </row>
     <row r="33" spans="2:6" ht="22" customHeight="1">
       <c r="B33" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E33" s="6"/>
       <c r="F33" s="7">
-        <v>940</v>
+        <v>585</v>
       </c>
     </row>
     <row r="34" spans="2:6" ht="22" customHeight="1">
       <c r="B34" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D34" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E34" s="6" t="s">
-        <v>42</v>
-      </c>
+      <c r="E34" s="6"/>
       <c r="F34" s="7">
-        <v>528</v>
+        <v>625</v>
       </c>
     </row>
     <row r="35" spans="2:6" ht="22" customHeight="1">
       <c r="B35" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D35" s="6" t="s">
         <v>32</v>
       </c>
       <c r="E35" s="6"/>
       <c r="F35" s="7">
-        <v>350</v>
+        <v>646</v>
       </c>
     </row>
     <row r="36" spans="2:6" ht="22" customHeight="1">
       <c r="B36" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E36" s="6"/>
       <c r="F36" s="7">
-        <v>940</v>
+        <v>654</v>
       </c>
     </row>
     <row r="37" spans="2:6" ht="22" customHeight="1">
       <c r="B37" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="E37" s="6"/>
       <c r="F37" s="7">
-        <v>330</v>
+        <v>677</v>
       </c>
     </row>
     <row r="38" spans="2:6" ht="22" customHeight="1">
       <c r="B38" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="E38" s="6"/>
       <c r="F38" s="7">
-        <v>490</v>
+        <v>680</v>
       </c>
     </row>
     <row r="39" spans="2:6" ht="22" customHeight="1">
       <c r="B39" s="5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E39" s="6"/>
       <c r="F39" s="7">
-        <v>540</v>
+        <v>690</v>
       </c>
     </row>
     <row r="40" spans="2:6" ht="22" customHeight="1">
       <c r="B40" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E40" s="6"/>
       <c r="F40" s="7">
-        <v>528</v>
+        <v>737</v>
       </c>
     </row>
     <row r="41" spans="2:6" ht="22" customHeight="1">
       <c r="B41" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="E41" s="6" t="s">
-        <v>42</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="E41" s="6"/>
       <c r="F41" s="7">
-        <v>156</v>
+        <v>737</v>
       </c>
     </row>
     <row r="42" spans="2:6" ht="22" customHeight="1">
       <c r="B42" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E42" s="6"/>
       <c r="F42" s="7">
-        <v>690</v>
+        <v>750</v>
       </c>
     </row>
     <row r="43" spans="2:6" ht="22" customHeight="1">
       <c r="B43" s="5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="E43" s="6" t="s">
-        <v>42</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="E43" s="6"/>
       <c r="F43" s="7">
-        <v>510</v>
+        <v>760</v>
       </c>
     </row>
     <row r="44" spans="2:6" ht="22" customHeight="1">
       <c r="B44" s="5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="E44" s="6"/>
       <c r="F44" s="7">
-        <v>536</v>
+        <v>760</v>
       </c>
     </row>
     <row r="45" spans="2:6" ht="22" customHeight="1">
       <c r="B45" s="5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E45" s="6"/>
       <c r="F45" s="7">
-        <v>760</v>
+        <v>810</v>
       </c>
     </row>
     <row r="46" spans="2:6" ht="22" customHeight="1">
       <c r="B46" s="5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="D46" s="6" t="s">
         <v>40</v>
       </c>
       <c r="E46" s="6"/>
       <c r="F46" s="7">
-        <v>172</v>
+        <v>918</v>
       </c>
     </row>
     <row r="47" spans="2:6" ht="22" customHeight="1">
       <c r="B47" s="5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E47" s="6"/>
       <c r="F47" s="7">
-        <v>1120</v>
+        <v>940</v>
       </c>
     </row>
     <row r="48" spans="2:6" ht="22" customHeight="1">
       <c r="B48" s="5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E48" s="6"/>
       <c r="F48" s="7">
-        <v>918</v>
+        <v>940</v>
       </c>
     </row>
     <row r="49" spans="2:6" ht="22" customHeight="1">
       <c r="B49" s="5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E49" s="6"/>
       <c r="F49" s="7">
-        <v>1398</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="50" spans="2:6" ht="22" customHeight="1">
       <c r="B50" s="5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E50" s="6"/>
       <c r="F50" s="7">
-        <v>810</v>
+        <v>1398</v>
       </c>
     </row>
   </sheetData>

</xml_diff>